<commit_message>
The fully functioning version we found some issues in VBA and corrected. Now it providing a strange output for the single species, because of light probably
</commit_message>
<xml_diff>
--- a/dev/input_data/input_eu_mixed.xlsx
+++ b/dev/input_data/input_eu_mixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A511E7CF-F5D2-2A42-A4FA-9617673F7CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D99308-87C7-F94D-BBA6-FD1679DEA93D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="6" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
+    <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="4" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="359">
   <si>
     <t>Name</t>
   </si>
@@ -1105,13 +1105,16 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>d13catm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1121,6 +1124,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1469,7 +1477,7 @@
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1479,7 +1487,7 @@
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>323</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1519,7 +1527,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1559,7 +1567,7 @@
         <v>0.1259168645351276</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1579,7 +1587,7 @@
         <v>2.2679</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1599,7 +1607,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1619,7 +1627,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1639,7 +1647,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1659,7 +1667,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1679,7 +1687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1719,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1759,7 +1767,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1779,7 +1787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1799,7 +1807,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1819,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1839,7 +1847,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1859,7 +1867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1879,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -1899,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1919,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1939,7 +1947,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1959,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1979,7 +1987,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1999,7 +2007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2019,7 +2027,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2039,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -2059,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -2079,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -2099,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2119,7 +2127,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2139,7 +2147,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2159,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2179,7 +2187,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2199,7 +2207,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -2219,7 +2227,7 @@
         <v>4.2920969347823963</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2239,7 +2247,7 @@
         <v>4.2920969347823963</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -2259,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -2279,7 +2287,7 @@
         <v>0.38277020142713869</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -2299,7 +2307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -2319,7 +2327,7 @@
         <v>0.39457142857142857</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -2339,7 +2347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>128</v>
       </c>
@@ -2359,7 +2367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>131</v>
       </c>
@@ -2379,7 +2387,7 @@
         <v>4.8565574202227367E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -2399,7 +2407,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -2419,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -2439,7 +2447,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -2459,7 +2467,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -2479,7 +2487,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>151</v>
       </c>
@@ -2499,7 +2507,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>154</v>
       </c>
@@ -2519,7 +2527,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -2539,7 +2547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>160</v>
       </c>
@@ -2559,7 +2567,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>163</v>
       </c>
@@ -2579,7 +2587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>166</v>
       </c>
@@ -2599,7 +2607,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>169</v>
       </c>
@@ -2619,7 +2627,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>172</v>
       </c>
@@ -2639,7 +2647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -2659,7 +2667,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>178</v>
       </c>
@@ -2679,7 +2687,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>181</v>
       </c>
@@ -2699,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -2719,7 +2727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>310</v>
       </c>
@@ -2739,7 +2747,7 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>313</v>
       </c>
@@ -2759,7 +2767,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>315</v>
       </c>
@@ -2776,7 +2784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>318</v>
       </c>
@@ -2806,9 +2814,9 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>323</v>
       </c>
@@ -2828,7 +2836,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -2848,7 +2856,7 @@
         <v>4.588685316132576</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -2868,7 +2876,7 @@
         <v>0.4738211</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>188</v>
       </c>
@@ -2888,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -2908,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>192</v>
       </c>
@@ -2928,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -2948,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>196</v>
       </c>
@@ -2968,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -2988,7 +2996,7 @@
         <v>1.3764906078875401</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>202</v>
       </c>
@@ -3008,7 +3016,7 @@
         <v>0.55362769999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>204</v>
       </c>
@@ -3028,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>206</v>
       </c>
@@ -3048,7 +3056,7 @@
         <v>-0.27724310000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -3065,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>210</v>
       </c>
@@ -3085,7 +3093,7 @@
         <v>2.1885791577597868</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>212</v>
       </c>
@@ -3105,7 +3113,7 @@
         <v>0.56325259999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -3125,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>216</v>
       </c>
@@ -3145,7 +3153,7 @@
         <v>-0.26567479999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -3162,7 +3170,7 @@
         <v>0.67789920000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>220</v>
       </c>
@@ -3182,7 +3190,7 @@
         <v>0.27800157495549827</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -3202,7 +3210,7 @@
         <v>1.1518027</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>226</v>
       </c>
@@ -3222,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>229</v>
       </c>
@@ -3242,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>232</v>
       </c>
@@ -3262,7 +3270,7 @@
         <v>5.4277699999999998E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>235</v>
       </c>
@@ -3282,7 +3290,7 @@
         <v>1.2283156000459392</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>238</v>
       </c>
@@ -3302,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>241</v>
       </c>
@@ -3322,7 +3330,7 @@
         <v>1.1889634</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>244</v>
       </c>
@@ -3342,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>247</v>
       </c>
@@ -3362,7 +3370,7 @@
         <v>0.2143678</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>250</v>
       </c>
@@ -3382,7 +3390,7 @@
         <v>0.98723714491917658</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>253</v>
       </c>
@@ -3402,7 +3410,7 @@
         <v>0.87204890000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>256</v>
       </c>
@@ -3422,7 +3430,7 @@
         <v>2.25852E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>259</v>
       </c>
@@ -3442,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>262</v>
       </c>
@@ -3462,7 +3470,7 @@
         <v>-0.10617219999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>265</v>
       </c>
@@ -3482,7 +3490,7 @@
         <v>9.0008110144060058E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>268</v>
       </c>
@@ -3502,7 +3510,7 @@
         <v>2.0841154999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>271</v>
       </c>
@@ -3522,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>274</v>
       </c>
@@ -3542,7 +3550,7 @@
         <v>0.27149630000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>277</v>
       </c>
@@ -3562,7 +3570,7 @@
         <v>-0.1222255</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>280</v>
       </c>
@@ -3582,7 +3590,7 @@
         <v>1.1339352444324555</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>283</v>
       </c>
@@ -3602,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>286</v>
       </c>
@@ -3622,7 +3630,7 @@
         <v>0.94494829999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>289</v>
       </c>
@@ -3642,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>292</v>
       </c>
@@ -3662,7 +3670,7 @@
         <v>0.12202789999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>295</v>
       </c>
@@ -3679,7 +3687,7 @@
         <v>0.22778889000228159</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>298</v>
       </c>
@@ -3696,7 +3704,7 @@
         <v>2.203662</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>301</v>
       </c>
@@ -3713,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>304</v>
       </c>
@@ -3730,7 +3738,7 @@
         <v>-0.41872100000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>307</v>
       </c>
@@ -3760,7 +3768,7 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3779,7 +3787,7 @@
     <col min="15" max="15" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>325</v>
       </c>
@@ -3805,7 +3813,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>50.11353888888889</v>
       </c>
@@ -3844,12 +3852,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>324</v>
       </c>
@@ -3875,7 +3883,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>321</v>
       </c>
@@ -3901,7 +3909,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" customHeight="1">
+    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -3934,15 +3942,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E86F09-F9D3-4B49-968A-3E0A41AAD9D8}">
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>344</v>
       </c>
@@ -3970,8 +3978,11 @@
       <c r="I1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2002</v>
       </c>
@@ -3997,10 +4008,13 @@
         <v>18</v>
       </c>
       <c r="I2">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>360</v>
+      </c>
+      <c r="J2">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -4026,10 +4040,13 @@
         <v>9</v>
       </c>
       <c r="I3">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>360.036</v>
+      </c>
+      <c r="J3">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -4055,10 +4072,13 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>360.07200360000002</v>
+      </c>
+      <c r="J4">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2002</v>
       </c>
@@ -4084,10 +4104,13 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>360.10801080036003</v>
+      </c>
+      <c r="J5">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -4113,10 +4136,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>360.14402160144004</v>
+      </c>
+      <c r="J6">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2002</v>
       </c>
@@ -4142,10 +4168,13 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>360.18003600360021</v>
+      </c>
+      <c r="J7">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2002</v>
       </c>
@@ -4171,10 +4200,13 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>360.21605400720057</v>
+      </c>
+      <c r="J8">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2002</v>
       </c>
@@ -4200,10 +4232,13 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>360.25207561260129</v>
+      </c>
+      <c r="J9">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -4229,10 +4264,13 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>360.28810082016253</v>
+      </c>
+      <c r="J10">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -4258,10 +4296,13 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>360.32412963024456</v>
+      </c>
+      <c r="J11">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -4287,10 +4328,13 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>360.36016204320759</v>
+      </c>
+      <c r="J12">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -4316,10 +4360,13 @@
         <v>14</v>
       </c>
       <c r="I13">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>360.39619805941192</v>
+      </c>
+      <c r="J13">
+        <v>-7.6778263499915012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2003</v>
       </c>
@@ -4345,10 +4392,13 @@
         <v>20</v>
       </c>
       <c r="I14">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>360.43223767921785</v>
+      </c>
+      <c r="J14">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -4374,10 +4424,13 @@
         <v>28</v>
       </c>
       <c r="I15">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>360.46828090298578</v>
+      </c>
+      <c r="J15">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -4403,10 +4456,13 @@
         <v>13</v>
       </c>
       <c r="I16">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>360.5043277310761</v>
+      </c>
+      <c r="J16">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -4432,10 +4488,13 @@
         <v>7</v>
       </c>
       <c r="I17">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>360.5403781638492</v>
+      </c>
+      <c r="J17">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -4461,10 +4520,13 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>360.57643220166557</v>
+      </c>
+      <c r="J18">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -4490,10 +4552,13 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>360.61248984488572</v>
+      </c>
+      <c r="J19">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2003</v>
       </c>
@@ -4519,10 +4584,13 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>360.6485510938702</v>
+      </c>
+      <c r="J20">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2003</v>
       </c>
@@ -4548,10 +4616,13 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>360.68461594897957</v>
+      </c>
+      <c r="J21">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2003</v>
       </c>
@@ -4577,10 +4648,13 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>360.72068441057445</v>
+      </c>
+      <c r="J22">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2003</v>
       </c>
@@ -4606,10 +4680,13 @@
         <v>6</v>
       </c>
       <c r="I23">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>360.75675647901551</v>
+      </c>
+      <c r="J23">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2003</v>
       </c>
@@ -4635,10 +4712,13 @@
         <v>3</v>
       </c>
       <c r="I24">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>360.79283215466342</v>
+      </c>
+      <c r="J24">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -4664,10 +4744,13 @@
         <v>19</v>
       </c>
       <c r="I25">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>360.8289114378789</v>
+      </c>
+      <c r="J25">
+        <v>-7.7052220501109474</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -4693,10 +4776,13 @@
         <v>21</v>
       </c>
       <c r="I26">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>360.86499432902269</v>
+      </c>
+      <c r="J26">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2004</v>
       </c>
@@ -4722,10 +4808,13 @@
         <v>17</v>
       </c>
       <c r="I27">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>360.90108082845558</v>
+      </c>
+      <c r="J27">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2004</v>
       </c>
@@ -4751,10 +4840,13 @@
         <v>17</v>
       </c>
       <c r="I28">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>360.93717093653839</v>
+      </c>
+      <c r="J28">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2004</v>
       </c>
@@ -4780,10 +4872,13 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>360.97326465363204</v>
+      </c>
+      <c r="J29">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2004</v>
       </c>
@@ -4809,10 +4904,13 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>361.00936198009742</v>
+      </c>
+      <c r="J30">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2004</v>
       </c>
@@ -4838,10 +4936,13 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>361.04546291629543</v>
+      </c>
+      <c r="J31">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2004</v>
       </c>
@@ -4867,10 +4968,13 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>361.08156746258709</v>
+      </c>
+      <c r="J32">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2004</v>
       </c>
@@ -4896,10 +5000,13 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>361.11767561933334</v>
+      </c>
+      <c r="J33">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2004</v>
       </c>
@@ -4925,10 +5032,13 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>361.15378738689526</v>
+      </c>
+      <c r="J34">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2004</v>
       </c>
@@ -4954,10 +5064,13 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>361.18990276563397</v>
+      </c>
+      <c r="J35">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -4983,10 +5096,13 @@
         <v>9</v>
       </c>
       <c r="I36">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>361.22602175591055</v>
+      </c>
+      <c r="J36">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2004</v>
       </c>
@@ -5012,10 +5128,13 @@
         <v>23</v>
       </c>
       <c r="I37">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>361.26214435808612</v>
+      </c>
+      <c r="J37">
+        <v>-7.7332187340141187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2005</v>
       </c>
@@ -5041,10 +5160,13 @@
         <v>15</v>
       </c>
       <c r="I38">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>361.29827057252191</v>
+      </c>
+      <c r="J38">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2005</v>
       </c>
@@ -5070,10 +5192,13 @@
         <v>25</v>
       </c>
       <c r="I39">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>361.33440039957918</v>
+      </c>
+      <c r="J39">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2005</v>
       </c>
@@ -5099,10 +5224,13 @@
         <v>13</v>
       </c>
       <c r="I40">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>361.37053383961916</v>
+      </c>
+      <c r="J40">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2005</v>
       </c>
@@ -5128,10 +5256,13 @@
         <v>1</v>
       </c>
       <c r="I41">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>361.40667089300314</v>
+      </c>
+      <c r="J41">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2005</v>
       </c>
@@ -5157,10 +5288,13 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>361.44281156009242</v>
+      </c>
+      <c r="J42">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2005</v>
       </c>
@@ -5186,10 +5320,13 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>361.47895584124842</v>
+      </c>
+      <c r="J43">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2005</v>
       </c>
@@ -5215,10 +5352,13 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>361.51510373683254</v>
+      </c>
+      <c r="J44">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2005</v>
       </c>
@@ -5244,10 +5384,13 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>361.5512552472062</v>
+      </c>
+      <c r="J45">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2005</v>
       </c>
@@ -5273,10 +5416,13 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>361.58741037273091</v>
+      </c>
+      <c r="J46">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2005</v>
       </c>
@@ -5302,10 +5448,13 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>361.62356911376816</v>
+      </c>
+      <c r="J47">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2005</v>
       </c>
@@ -5331,10 +5480,13 @@
         <v>10</v>
       </c>
       <c r="I48">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>361.6597314706795</v>
+      </c>
+      <c r="J48">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2005</v>
       </c>
@@ -5360,10 +5512,13 @@
         <v>18</v>
       </c>
       <c r="I49">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>361.6958974438266</v>
+      </c>
+      <c r="J49">
+        <v>-7.7618295855768338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2006</v>
       </c>
@@ -5389,10 +5544,13 @@
         <v>26</v>
       </c>
       <c r="I50">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>361.73206703357096</v>
+      </c>
+      <c r="J50">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2006</v>
       </c>
@@ -5418,10 +5576,13 @@
         <v>20</v>
       </c>
       <c r="I51">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>361.76824024027434</v>
+      </c>
+      <c r="J51">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2006</v>
       </c>
@@ -5447,10 +5608,13 @@
         <v>22</v>
       </c>
       <c r="I52">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>361.80441706429838</v>
+      </c>
+      <c r="J52">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2006</v>
       </c>
@@ -5476,10 +5640,13 @@
         <v>2</v>
       </c>
       <c r="I53">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>361.84059750600483</v>
+      </c>
+      <c r="J53">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2006</v>
       </c>
@@ -5505,10 +5672,13 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>361.87678156575544</v>
+      </c>
+      <c r="J54">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2006</v>
       </c>
@@ -5534,10 +5704,13 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>361.91296924391202</v>
+      </c>
+      <c r="J55">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2006</v>
       </c>
@@ -5563,10 +5736,13 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>361.94916054083643</v>
+      </c>
+      <c r="J56">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2006</v>
       </c>
@@ -5592,10 +5768,13 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>361.98535545689049</v>
+      </c>
+      <c r="J57">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2006</v>
       </c>
@@ -5621,10 +5800,13 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>362.02155399243617</v>
+      </c>
+      <c r="J58">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2006</v>
       </c>
@@ -5650,10 +5832,13 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>362.05775614783539</v>
+      </c>
+      <c r="J59">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2006</v>
       </c>
@@ -5679,10 +5864,13 @@
         <v>1</v>
       </c>
       <c r="I60">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>362.09396192345019</v>
+      </c>
+      <c r="J60">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2006</v>
       </c>
@@ -5708,10 +5896,13 @@
         <v>11</v>
       </c>
       <c r="I61">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>362.13017131964256</v>
+      </c>
+      <c r="J61">
+        <v>-7.7910680778916674</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2007</v>
       </c>
@@ -5737,10 +5928,13 @@
         <v>8</v>
       </c>
       <c r="I62">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>362.16638433677451</v>
+      </c>
+      <c r="J62">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2007</v>
       </c>
@@ -5766,10 +5960,13 @@
         <v>12</v>
       </c>
       <c r="I63">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>362.20260097520821</v>
+      </c>
+      <c r="J63">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2007</v>
       </c>
@@ -5795,10 +5992,13 @@
         <v>4</v>
       </c>
       <c r="I64">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>362.23882123530575</v>
+      </c>
+      <c r="J64">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2007</v>
       </c>
@@ -5824,10 +6024,13 @@
         <v>1</v>
       </c>
       <c r="I65">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>362.27504511742927</v>
+      </c>
+      <c r="J65">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2007</v>
       </c>
@@ -5853,10 +6056,13 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>362.31127262194099</v>
+      </c>
+      <c r="J66">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2007</v>
       </c>
@@ -5882,10 +6088,13 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>362.34750374920316</v>
+      </c>
+      <c r="J67">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2007</v>
       </c>
@@ -5911,10 +6120,13 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>362.3837384995781</v>
+      </c>
+      <c r="J68">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2007</v>
       </c>
@@ -5940,10 +6152,13 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>362.41997687342803</v>
+      </c>
+      <c r="J69">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2007</v>
       </c>
@@ -5969,10 +6184,13 @@
         <v>0</v>
       </c>
       <c r="I70">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>362.45621887111537</v>
+      </c>
+      <c r="J70">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2007</v>
       </c>
@@ -5998,10 +6216,13 @@
         <v>0</v>
       </c>
       <c r="I71">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>362.4924644930025</v>
+      </c>
+      <c r="J71">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2007</v>
       </c>
@@ -6027,10 +6248,13 @@
         <v>10</v>
       </c>
       <c r="I72">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>362.5287137394518</v>
+      </c>
+      <c r="J72">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2007</v>
       </c>
@@ -6056,10 +6280,13 @@
         <v>18</v>
       </c>
       <c r="I73">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>362.56496661082576</v>
+      </c>
+      <c r="J73">
+        <v>-7.820947979612547</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2008</v>
       </c>
@@ -6085,10 +6312,13 @@
         <v>10</v>
       </c>
       <c r="I74">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>362.60122310748682</v>
+      </c>
+      <c r="J74">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2008</v>
       </c>
@@ -6114,10 +6344,13 @@
         <v>17</v>
       </c>
       <c r="I75">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>362.63748322979757</v>
+      </c>
+      <c r="J75">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2008</v>
       </c>
@@ -6143,10 +6376,13 @@
         <v>10</v>
       </c>
       <c r="I76">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>362.67374697812056</v>
+      </c>
+      <c r="J76">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2008</v>
       </c>
@@ -6172,10 +6408,13 @@
         <v>3</v>
       </c>
       <c r="I77">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+        <v>362.71001435281835</v>
+      </c>
+      <c r="J77">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2008</v>
       </c>
@@ -6201,10 +6440,13 @@
         <v>0</v>
       </c>
       <c r="I78">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>362.74628535425364</v>
+      </c>
+      <c r="J78">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2008</v>
       </c>
@@ -6230,10 +6472,13 @@
         <v>0</v>
       </c>
       <c r="I79">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>362.78255998278905</v>
+      </c>
+      <c r="J79">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2008</v>
       </c>
@@ -6259,10 +6504,13 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+        <v>362.81883823878735</v>
+      </c>
+      <c r="J80">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2008</v>
       </c>
@@ -6288,10 +6536,13 @@
         <v>0</v>
       </c>
       <c r="I81">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+        <v>362.8551201226112</v>
+      </c>
+      <c r="J81">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2008</v>
       </c>
@@ -6317,10 +6568,13 @@
         <v>0</v>
       </c>
       <c r="I82">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+        <v>362.89140563462348</v>
+      </c>
+      <c r="J82">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2008</v>
       </c>
@@ -6346,10 +6600,13 @@
         <v>1</v>
       </c>
       <c r="I83">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+        <v>362.92769477518692</v>
+      </c>
+      <c r="J83">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2008</v>
       </c>
@@ -6375,10 +6632,13 @@
         <v>11</v>
       </c>
       <c r="I84">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+        <v>362.96398754466446</v>
+      </c>
+      <c r="J84">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2008</v>
       </c>
@@ -6404,10 +6664,13 @@
         <v>19</v>
       </c>
       <c r="I85">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+        <v>363.00028394341894</v>
+      </c>
+      <c r="J85">
+        <v>-7.8514833614385262</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2009</v>
       </c>
@@ -6433,10 +6696,13 @@
         <v>29</v>
       </c>
       <c r="I86">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+        <v>363.03658397181329</v>
+      </c>
+      <c r="J86">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2009</v>
       </c>
@@ -6462,10 +6728,13 @@
         <v>22</v>
       </c>
       <c r="I87">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+        <v>363.07288763021046</v>
+      </c>
+      <c r="J87">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2009</v>
       </c>
@@ -6491,10 +6760,13 @@
         <v>9</v>
       </c>
       <c r="I88">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+        <v>363.10919491897346</v>
+      </c>
+      <c r="J88">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2009</v>
       </c>
@@ -6520,10 +6792,13 @@
         <v>0</v>
       </c>
       <c r="I89">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+        <v>363.14550583846534</v>
+      </c>
+      <c r="J89">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2009</v>
       </c>
@@ -6549,10 +6824,13 @@
         <v>0</v>
       </c>
       <c r="I90">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+        <v>363.18182038904916</v>
+      </c>
+      <c r="J90">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2009</v>
       </c>
@@ -6578,10 +6856,13 @@
         <v>0</v>
       </c>
       <c r="I91">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+        <v>363.21813857108805</v>
+      </c>
+      <c r="J91">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2009</v>
       </c>
@@ -6607,10 +6888,13 @@
         <v>0</v>
       </c>
       <c r="I92">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+        <v>363.25446038494516</v>
+      </c>
+      <c r="J92">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2009</v>
       </c>
@@ -6636,10 +6920,13 @@
         <v>0</v>
       </c>
       <c r="I93">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+        <v>363.29078583098368</v>
+      </c>
+      <c r="J93">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2009</v>
       </c>
@@ -6665,10 +6952,13 @@
         <v>0</v>
       </c>
       <c r="I94">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+        <v>363.32711490956677</v>
+      </c>
+      <c r="J94">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2009</v>
       </c>
@@ -6694,10 +6984,13 @@
         <v>2</v>
       </c>
       <c r="I95">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+        <v>363.36344762105773</v>
+      </c>
+      <c r="J95">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2009</v>
       </c>
@@ -6723,10 +7016,13 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>363.39978396581984</v>
+      </c>
+      <c r="J96">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2009</v>
       </c>
@@ -6752,10 +7048,13 @@
         <v>16</v>
       </c>
       <c r="I97">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>363.43612394421643</v>
+      </c>
+      <c r="J97">
+        <v>-7.8826886027397975</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2010</v>
       </c>
@@ -6781,10 +7080,13 @@
         <v>29</v>
       </c>
       <c r="I98">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+        <v>363.47246755661087</v>
+      </c>
+      <c r="J98">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2010</v>
       </c>
@@ -6810,10 +7112,13 @@
         <v>22</v>
       </c>
       <c r="I99">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+        <v>363.50881480336653</v>
+      </c>
+      <c r="J99">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2010</v>
       </c>
@@ -6839,10 +7144,13 @@
         <v>15</v>
       </c>
       <c r="I100">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+        <v>363.54516568484689</v>
+      </c>
+      <c r="J100">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2010</v>
       </c>
@@ -6868,10 +7176,13 @@
         <v>2</v>
       </c>
       <c r="I101">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+        <v>363.5815202014154</v>
+      </c>
+      <c r="J101">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2010</v>
       </c>
@@ -6897,10 +7208,13 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+        <v>363.61787835343551</v>
+      </c>
+      <c r="J102">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2010</v>
       </c>
@@ -6926,10 +7240,13 @@
         <v>0</v>
       </c>
       <c r="I103">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+        <v>363.65424014127086</v>
+      </c>
+      <c r="J103">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2010</v>
       </c>
@@ -6955,10 +7272,13 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+        <v>363.69060556528501</v>
+      </c>
+      <c r="J104">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2010</v>
       </c>
@@ -6984,10 +7304,13 @@
         <v>0</v>
       </c>
       <c r="I105">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+        <v>363.72697462584154</v>
+      </c>
+      <c r="J105">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2010</v>
       </c>
@@ -7013,10 +7336,13 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+        <v>363.76334732330412</v>
+      </c>
+      <c r="J106">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2010</v>
       </c>
@@ -7042,10 +7368,13 @@
         <v>4</v>
       </c>
       <c r="I107">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+        <v>363.79972365803644</v>
+      </c>
+      <c r="J107">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2010</v>
       </c>
@@ -7071,10 +7400,13 @@
         <v>5</v>
       </c>
       <c r="I108">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
+        <v>363.83610363040225</v>
+      </c>
+      <c r="J108">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2010</v>
       </c>
@@ -7100,10 +7432,13 @@
         <v>30</v>
       </c>
       <c r="I109">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
+        <v>363.87248724076528</v>
+      </c>
+      <c r="J109">
+        <v>-7.9145783983290627</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2011</v>
       </c>
@@ -7129,10 +7464,13 @@
         <v>20</v>
       </c>
       <c r="I110">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+        <v>363.90887448948934</v>
+      </c>
+      <c r="J110">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2011</v>
       </c>
@@ -7158,10 +7496,13 @@
         <v>20</v>
       </c>
       <c r="I111">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
+        <v>363.94526537693827</v>
+      </c>
+      <c r="J111">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2011</v>
       </c>
@@ -7187,10 +7528,13 @@
         <v>12</v>
       </c>
       <c r="I112">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+        <v>363.98165990347593</v>
+      </c>
+      <c r="J112">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2011</v>
       </c>
@@ -7216,10 +7560,13 @@
         <v>0</v>
       </c>
       <c r="I113">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
+        <v>364.01805806946629</v>
+      </c>
+      <c r="J113">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2011</v>
       </c>
@@ -7245,10 +7592,13 @@
         <v>0</v>
       </c>
       <c r="I114">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+        <v>364.05445987527321</v>
+      </c>
+      <c r="J114">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2011</v>
       </c>
@@ -7274,10 +7624,13 @@
         <v>0</v>
       </c>
       <c r="I115">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+        <v>364.09086532126071</v>
+      </c>
+      <c r="J115">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2011</v>
       </c>
@@ -7303,10 +7656,13 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+        <v>364.12727440779281</v>
+      </c>
+      <c r="J116">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2011</v>
       </c>
@@ -7332,10 +7688,13 @@
         <v>0</v>
       </c>
       <c r="I117">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+        <v>364.1636871352336</v>
+      </c>
+      <c r="J117">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2011</v>
       </c>
@@ -7361,10 +7720,13 @@
         <v>0</v>
       </c>
       <c r="I118">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+        <v>364.2001035039471</v>
+      </c>
+      <c r="J118">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2011</v>
       </c>
@@ -7390,10 +7752,13 @@
         <v>3</v>
       </c>
       <c r="I119">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+        <v>364.23652351429752</v>
+      </c>
+      <c r="J119">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2011</v>
       </c>
@@ -7419,10 +7784,13 @@
         <v>14</v>
       </c>
       <c r="I120">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v>364.27294716664892</v>
+      </c>
+      <c r="J120">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2011</v>
       </c>
@@ -7448,10 +7816,13 @@
         <v>6</v>
       </c>
       <c r="I121">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+        <v>364.30937446136556</v>
+      </c>
+      <c r="J121">
+        <v>-7.9471677653814368</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2012</v>
       </c>
@@ -7477,10 +7848,13 @@
         <v>13</v>
       </c>
       <c r="I122">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>364.34580539881171</v>
+      </c>
+      <c r="J122">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>2012</v>
       </c>
@@ -7506,10 +7880,13 @@
         <v>19</v>
       </c>
       <c r="I123">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
+        <v>364.3822399793516</v>
+      </c>
+      <c r="J123">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2012</v>
       </c>
@@ -7535,10 +7912,13 @@
         <v>8</v>
       </c>
       <c r="I124">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+        <v>364.41867820334954</v>
+      </c>
+      <c r="J124">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2012</v>
       </c>
@@ -7564,10 +7944,13 @@
         <v>4</v>
       </c>
       <c r="I125">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+        <v>364.45512007116986</v>
+      </c>
+      <c r="J125">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2012</v>
       </c>
@@ -7593,10 +7976,13 @@
         <v>0</v>
       </c>
       <c r="I126">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+        <v>364.49156558317696</v>
+      </c>
+      <c r="J126">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2012</v>
       </c>
@@ -7622,10 +8008,13 @@
         <v>0</v>
       </c>
       <c r="I127">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+        <v>364.52801473973528</v>
+      </c>
+      <c r="J127">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2012</v>
       </c>
@@ -7651,10 +8040,13 @@
         <v>0</v>
       </c>
       <c r="I128">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
+        <v>364.56446754120924</v>
+      </c>
+      <c r="J128">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2012</v>
       </c>
@@ -7680,10 +8072,13 @@
         <v>0</v>
       </c>
       <c r="I129">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
+        <v>364.60092398796337</v>
+      </c>
+      <c r="J129">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2012</v>
       </c>
@@ -7709,10 +8104,13 @@
         <v>0</v>
       </c>
       <c r="I130">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
+        <v>364.63738408036215</v>
+      </c>
+      <c r="J130">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2012</v>
       </c>
@@ -7738,10 +8136,13 @@
         <v>2</v>
       </c>
       <c r="I131">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
+        <v>364.67384781877018</v>
+      </c>
+      <c r="J131">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2012</v>
       </c>
@@ -7767,10 +8168,13 @@
         <v>8</v>
       </c>
       <c r="I132">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
+        <v>364.71031520355206</v>
+      </c>
+      <c r="J132">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2012</v>
       </c>
@@ -7796,10 +8200,13 @@
         <v>14</v>
       </c>
       <c r="I133">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9">
+        <v>364.74678623507242</v>
+      </c>
+      <c r="J133">
+        <v>-7.9804720505061724</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>2013</v>
       </c>
@@ -7825,10 +8232,13 @@
         <v>18</v>
       </c>
       <c r="I134">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
+        <v>364.78326091369593</v>
+      </c>
+      <c r="J134">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2013</v>
       </c>
@@ -7854,10 +8264,13 @@
         <v>26</v>
       </c>
       <c r="I135">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
+        <v>364.81973923978728</v>
+      </c>
+      <c r="J135">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2013</v>
       </c>
@@ -7883,10 +8296,13 @@
         <v>26</v>
       </c>
       <c r="I136">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
+        <v>364.85622121371125</v>
+      </c>
+      <c r="J136">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2013</v>
       </c>
@@ -7912,10 +8328,13 @@
         <v>7</v>
       </c>
       <c r="I137">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
+        <v>364.8927068358326</v>
+      </c>
+      <c r="J137">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2013</v>
       </c>
@@ -7941,10 +8360,13 @@
         <v>0</v>
       </c>
       <c r="I138">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
+        <v>364.9291961065162</v>
+      </c>
+      <c r="J138">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2013</v>
       </c>
@@ -7970,10 +8392,13 @@
         <v>0</v>
       </c>
       <c r="I139">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9">
+        <v>364.96568902612682</v>
+      </c>
+      <c r="J139">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2013</v>
       </c>
@@ -7999,10 +8424,13 @@
         <v>0</v>
       </c>
       <c r="I140">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9">
+        <v>365.00218559502946</v>
+      </c>
+      <c r="J140">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2013</v>
       </c>
@@ -8028,10 +8456,13 @@
         <v>0</v>
       </c>
       <c r="I141">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9">
+        <v>365.03868581358898</v>
+      </c>
+      <c r="J141">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2013</v>
       </c>
@@ -8057,10 +8488,13 @@
         <v>0</v>
       </c>
       <c r="I142">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9">
+        <v>365.07518968217033</v>
+      </c>
+      <c r="J142">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2013</v>
       </c>
@@ -8086,10 +8520,13 @@
         <v>1</v>
       </c>
       <c r="I143">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9">
+        <v>365.11169720113855</v>
+      </c>
+      <c r="J143">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2013</v>
       </c>
@@ -8115,10 +8552,13 @@
         <v>8</v>
       </c>
       <c r="I144">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9">
+        <v>365.14820837085864</v>
+      </c>
+      <c r="J144">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2013</v>
       </c>
@@ -8144,10 +8584,13 @@
         <v>11</v>
       </c>
       <c r="I145">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9">
+        <v>365.1847231916957</v>
+      </c>
+      <c r="J145">
+        <v>-8.0145069369735005</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2014</v>
       </c>
@@ -8173,10 +8616,13 @@
         <v>10</v>
       </c>
       <c r="I146">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9">
+        <v>365.22124166401488</v>
+      </c>
+      <c r="J146">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2014</v>
       </c>
@@ -8202,10 +8648,13 @@
         <v>7</v>
       </c>
       <c r="I147">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9">
+        <v>365.25776378818131</v>
+      </c>
+      <c r="J147">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2014</v>
       </c>
@@ -8231,10 +8680,13 @@
         <v>5</v>
       </c>
       <c r="I148">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9">
+        <v>365.29428956456013</v>
+      </c>
+      <c r="J148">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2014</v>
       </c>
@@ -8260,10 +8712,13 @@
         <v>0</v>
       </c>
       <c r="I149">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9">
+        <v>365.33081899351657</v>
+      </c>
+      <c r="J149">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2014</v>
       </c>
@@ -8289,10 +8744,13 @@
         <v>0</v>
       </c>
       <c r="I150">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9">
+        <v>365.36735207541591</v>
+      </c>
+      <c r="J150">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2014</v>
       </c>
@@ -8318,10 +8776,13 @@
         <v>0</v>
       </c>
       <c r="I151">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9">
+        <v>365.40388881062347</v>
+      </c>
+      <c r="J151">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2014</v>
       </c>
@@ -8347,10 +8808,13 @@
         <v>0</v>
       </c>
       <c r="I152">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9">
+        <v>365.44042919950454</v>
+      </c>
+      <c r="J152">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2014</v>
       </c>
@@ -8376,10 +8840,13 @@
         <v>0</v>
       </c>
       <c r="I153">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9">
+        <v>365.47697324242449</v>
+      </c>
+      <c r="J153">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -8405,10 +8872,13 @@
         <v>0</v>
       </c>
       <c r="I154">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9">
+        <v>365.51352093974873</v>
+      </c>
+      <c r="J154">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -8434,10 +8904,13 @@
         <v>0</v>
       </c>
       <c r="I155">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9">
+        <v>365.5500722918427</v>
+      </c>
+      <c r="J155">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -8463,10 +8936,13 @@
         <v>4</v>
       </c>
       <c r="I156">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9">
+        <v>365.58662729907189</v>
+      </c>
+      <c r="J156">
+        <v>-8.0492884521000221</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -8492,7 +8968,10 @@
         <v>11</v>
       </c>
       <c r="I157">
-        <v>350</v>
+        <v>365.62318596180182</v>
+      </c>
+      <c r="J157">
+        <v>-8.0492884521000221</v>
       </c>
     </row>
   </sheetData>
@@ -8508,9 +8987,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>336</v>
       </c>
@@ -8530,7 +9009,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>342</v>
       </c>
@@ -8556,13 +9035,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3ED633-EED0-A541-B1D7-08B1459B1DF2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>353</v>
       </c>
@@ -8579,7 +9058,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>999</v>
       </c>

</xml_diff>

<commit_message>
Monospecies without bias are working great! `Climate` output done
</commit_message>
<xml_diff>
--- a/dev/input_data/input_eu_mixed.xlsx
+++ b/dev/input_data/input_eu_mixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D99308-87C7-F94D-BBA6-FD1679DEA93D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D220B0B-9939-C24F-8542-07FFA896AAE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="4" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
   </bookViews>
@@ -1114,7 +1114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1124,11 +1124,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1154,8 +1149,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1474,7 +1470,7 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,7 +1480,7 @@
     <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1503,7 +1499,7 @@
       <c r="E1" t="s">
         <v>321</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>322</v>
       </c>
     </row>
@@ -1523,7 +1519,7 @@
       <c r="E2">
         <v>0.7</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -1543,7 +1539,7 @@
       <c r="E3">
         <v>0.06</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.21</v>
       </c>
     </row>
@@ -1563,7 +1559,7 @@
       <c r="E4">
         <v>0.18338848112302766</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.1259168645351276</v>
       </c>
     </row>
@@ -1583,7 +1579,7 @@
       <c r="E5">
         <v>2.3895</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>2.2679</v>
       </c>
     </row>
@@ -1603,7 +1599,7 @@
       <c r="E6">
         <v>0.7</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -1623,7 +1619,7 @@
       <c r="E7">
         <v>0.3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0.3</v>
       </c>
     </row>
@@ -1643,7 +1639,7 @@
       <c r="E8">
         <v>0.02</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -1663,7 +1659,7 @@
       <c r="E9">
         <v>1E-3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>1E-3</v>
       </c>
     </row>
@@ -1683,7 +1679,7 @@
       <c r="E10">
         <v>60</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>60</v>
       </c>
     </row>
@@ -1703,7 +1699,7 @@
       <c r="E11">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -1723,7 +1719,7 @@
       <c r="E12">
         <v>4</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1743,7 +1739,7 @@
       <c r="E13">
         <v>11</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1763,7 +1759,7 @@
       <c r="E14">
         <v>-5</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>-5</v>
       </c>
     </row>
@@ -1783,7 +1779,7 @@
       <c r="E15">
         <v>20</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>15</v>
       </c>
     </row>
@@ -1803,7 +1799,7 @@
       <c r="E16">
         <v>25</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>35</v>
       </c>
     </row>
@@ -1823,7 +1819,7 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1843,7 +1839,7 @@
       <c r="E18">
         <v>0.7</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -1863,7 +1859,7 @@
       <c r="E19">
         <v>9</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1883,7 +1879,7 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1903,7 +1899,7 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1923,7 +1919,7 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1943,7 +1939,7 @@
       <c r="E23">
         <v>0.5</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -1963,7 +1959,7 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1983,7 +1979,7 @@
       <c r="E25">
         <v>300</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>350</v>
       </c>
     </row>
@@ -2003,7 +1999,7 @@
       <c r="E26">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>4</v>
       </c>
     </row>
@@ -2023,7 +2019,7 @@
       <c r="E27">
         <v>0.95</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>0.95</v>
       </c>
     </row>
@@ -2043,7 +2039,7 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2063,7 +2059,7 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2083,7 +2079,7 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2103,7 +2099,7 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2123,7 +2119,7 @@
       <c r="E32">
         <v>400</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>400</v>
       </c>
     </row>
@@ -2143,7 +2139,7 @@
       <c r="E33">
         <v>1.5</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>1.5</v>
       </c>
     </row>
@@ -2163,7 +2159,7 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2183,7 +2179,7 @@
       <c r="E35">
         <v>0.2</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -2203,7 +2199,7 @@
       <c r="E36">
         <v>0.4</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -2223,7 +2219,7 @@
       <c r="E37">
         <v>24.718999411782914</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>4.2920969347823963</v>
       </c>
     </row>
@@ -2243,7 +2239,7 @@
       <c r="E38">
         <v>19.402050203937655</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>4.2920969347823963</v>
       </c>
     </row>
@@ -2263,7 +2259,7 @@
       <c r="E39">
         <v>35</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2283,7 +2279,7 @@
       <c r="E40">
         <v>0.41781825591268146</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>0.38277020142713869</v>
       </c>
     </row>
@@ -2303,7 +2299,7 @@
       <c r="E41">
         <v>10</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>10</v>
       </c>
     </row>
@@ -2323,7 +2319,7 @@
       <c r="E42">
         <v>0.23733333333333331</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>0.39457142857142857</v>
       </c>
     </row>
@@ -2343,7 +2339,7 @@
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2363,7 +2359,7 @@
       <c r="E44">
         <v>5</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>5</v>
       </c>
     </row>
@@ -2383,7 +2379,7 @@
       <c r="E45">
         <v>4.9810073254773303E-2</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>4.8565574202227367E-2</v>
       </c>
     </row>
@@ -2403,7 +2399,7 @@
       <c r="E46">
         <v>0.47</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>0.47</v>
       </c>
     </row>
@@ -2423,7 +2419,7 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2443,7 +2439,7 @@
       <c r="E48">
         <v>0.02</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>0.02</v>
       </c>
     </row>
@@ -2463,7 +2459,7 @@
       <c r="E49">
         <v>3.33</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>3.33</v>
       </c>
     </row>
@@ -2483,7 +2479,7 @@
       <c r="E50">
         <v>5.6999999999999995E-2</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>0.05</v>
       </c>
     </row>
@@ -2503,7 +2499,7 @@
       <c r="E51">
         <v>0.2</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <v>0.2</v>
       </c>
     </row>
@@ -2523,7 +2519,7 @@
       <c r="E52">
         <v>0.66</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <v>0.66</v>
       </c>
     </row>
@@ -2543,7 +2539,7 @@
       <c r="E53">
         <v>2</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2563,7 +2559,7 @@
       <c r="E54">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2583,7 +2579,7 @@
       <c r="E55">
         <v>27</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="1">
         <v>27</v>
       </c>
     </row>
@@ -2603,7 +2599,7 @@
       <c r="E56">
         <v>0.75</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <v>0.75</v>
       </c>
     </row>
@@ -2623,7 +2619,7 @@
       <c r="E57">
         <v>0.15</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="1">
         <v>0.15</v>
       </c>
     </row>
@@ -2643,7 +2639,7 @@
       <c r="E58">
         <v>2</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2663,7 +2659,7 @@
       <c r="E59">
         <v>0.56699999999999995</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <v>0.39500000000000002</v>
       </c>
     </row>
@@ -2683,7 +2679,7 @@
       <c r="E60">
         <v>0.56699999999999995</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="1">
         <v>0.39500000000000002</v>
       </c>
     </row>
@@ -2703,7 +2699,7 @@
       <c r="E61">
         <v>1</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2723,7 +2719,7 @@
       <c r="E62">
         <v>3</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2743,7 +2739,7 @@
       <c r="E63">
         <v>-90</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="1">
         <v>-90</v>
       </c>
     </row>
@@ -2763,7 +2759,7 @@
       <c r="E64">
         <v>0.8</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="1">
         <v>0.8</v>
       </c>
     </row>
@@ -2780,7 +2776,7 @@
       <c r="E65">
         <v>24</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="1">
         <v>24</v>
       </c>
     </row>
@@ -2797,7 +2793,7 @@
       <c r="E66">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="1">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -3944,8 +3940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E86F09-F9D3-4B49-968A-3E0A41AAD9D8}">
   <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="M145" sqref="M145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4008,10 +4004,10 @@
         <v>18</v>
       </c>
       <c r="I2">
-        <v>360</v>
+        <v>360.43223767921785</v>
       </c>
       <c r="J2">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -4040,10 +4036,10 @@
         <v>9</v>
       </c>
       <c r="I3">
-        <v>360.036</v>
+        <v>360.46828090298578</v>
       </c>
       <c r="J3">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -4072,10 +4068,10 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <v>360.07200360000002</v>
+        <v>360.5043277310761</v>
       </c>
       <c r="J4">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -4104,10 +4100,10 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>360.10801080036003</v>
+        <v>360.5403781638492</v>
       </c>
       <c r="J5">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -4136,10 +4132,10 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>360.14402160144004</v>
+        <v>360.57643220166557</v>
       </c>
       <c r="J6">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -4168,10 +4164,10 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>360.18003600360021</v>
+        <v>360.61248984488572</v>
       </c>
       <c r="J7">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -4200,10 +4196,10 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>360.21605400720057</v>
+        <v>360.6485510938702</v>
       </c>
       <c r="J8">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -4232,10 +4228,10 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>360.25207561260129</v>
+        <v>360.68461594897957</v>
       </c>
       <c r="J9">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -4264,10 +4260,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>360.28810082016253</v>
+        <v>360.72068441057445</v>
       </c>
       <c r="J10">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -4296,10 +4292,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>360.32412963024456</v>
+        <v>360.75675647901551</v>
       </c>
       <c r="J11">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -4328,10 +4324,10 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>360.36016204320759</v>
+        <v>360.79283215466342</v>
       </c>
       <c r="J12">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -4360,10 +4356,10 @@
         <v>14</v>
       </c>
       <c r="I13">
-        <v>360.39619805941192</v>
+        <v>360.8289114378789</v>
       </c>
       <c r="J13">
-        <v>-7.6778263499915012</v>
+        <v>-7.7052220501109474</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -4392,10 +4388,10 @@
         <v>20</v>
       </c>
       <c r="I14">
-        <v>360.43223767921785</v>
+        <v>360.86499432902269</v>
       </c>
       <c r="J14">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -4424,10 +4420,10 @@
         <v>28</v>
       </c>
       <c r="I15">
-        <v>360.46828090298578</v>
+        <v>360.90108082845558</v>
       </c>
       <c r="J15">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -4456,10 +4452,10 @@
         <v>13</v>
       </c>
       <c r="I16">
-        <v>360.5043277310761</v>
+        <v>360.93717093653839</v>
       </c>
       <c r="J16">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -4488,10 +4484,10 @@
         <v>7</v>
       </c>
       <c r="I17">
-        <v>360.5403781638492</v>
+        <v>360.97326465363204</v>
       </c>
       <c r="J17">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -4520,10 +4516,10 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>360.57643220166557</v>
+        <v>361.00936198009742</v>
       </c>
       <c r="J18">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -4552,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>360.61248984488572</v>
+        <v>361.04546291629543</v>
       </c>
       <c r="J19">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -4584,10 +4580,10 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>360.6485510938702</v>
+        <v>361.08156746258709</v>
       </c>
       <c r="J20">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -4616,10 +4612,10 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>360.68461594897957</v>
+        <v>361.11767561933334</v>
       </c>
       <c r="J21">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -4648,10 +4644,10 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>360.72068441057445</v>
+        <v>361.15378738689526</v>
       </c>
       <c r="J22">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -4680,10 +4676,10 @@
         <v>6</v>
       </c>
       <c r="I23">
-        <v>360.75675647901551</v>
+        <v>361.18990276563397</v>
       </c>
       <c r="J23">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -4712,10 +4708,10 @@
         <v>3</v>
       </c>
       <c r="I24">
-        <v>360.79283215466342</v>
+        <v>361.22602175591055</v>
       </c>
       <c r="J24">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -4744,10 +4740,10 @@
         <v>19</v>
       </c>
       <c r="I25">
-        <v>360.8289114378789</v>
+        <v>361.26214435808612</v>
       </c>
       <c r="J25">
-        <v>-7.7052220501109474</v>
+        <v>-7.7332187340141187</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -4776,10 +4772,10 @@
         <v>21</v>
       </c>
       <c r="I26">
-        <v>360.86499432902269</v>
+        <v>361.29827057252191</v>
       </c>
       <c r="J26">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -4808,10 +4804,10 @@
         <v>17</v>
       </c>
       <c r="I27">
-        <v>360.90108082845558</v>
+        <v>361.33440039957918</v>
       </c>
       <c r="J27">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -4840,10 +4836,10 @@
         <v>17</v>
       </c>
       <c r="I28">
-        <v>360.93717093653839</v>
+        <v>361.37053383961916</v>
       </c>
       <c r="J28">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -4872,10 +4868,10 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <v>360.97326465363204</v>
+        <v>361.40667089300314</v>
       </c>
       <c r="J29">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -4904,10 +4900,10 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>361.00936198009742</v>
+        <v>361.44281156009242</v>
       </c>
       <c r="J30">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -4936,10 +4932,10 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>361.04546291629543</v>
+        <v>361.47895584124842</v>
       </c>
       <c r="J31">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -4968,10 +4964,10 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>361.08156746258709</v>
+        <v>361.51510373683254</v>
       </c>
       <c r="J32">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -5000,10 +4996,10 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>361.11767561933334</v>
+        <v>361.5512552472062</v>
       </c>
       <c r="J33">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -5032,10 +5028,10 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>361.15378738689526</v>
+        <v>361.58741037273091</v>
       </c>
       <c r="J34">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -5064,10 +5060,10 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>361.18990276563397</v>
+        <v>361.62356911376816</v>
       </c>
       <c r="J35">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -5096,10 +5092,10 @@
         <v>9</v>
       </c>
       <c r="I36">
-        <v>361.22602175591055</v>
+        <v>361.6597314706795</v>
       </c>
       <c r="J36">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -5128,10 +5124,10 @@
         <v>23</v>
       </c>
       <c r="I37">
-        <v>361.26214435808612</v>
+        <v>361.6958974438266</v>
       </c>
       <c r="J37">
-        <v>-7.7332187340141187</v>
+        <v>-7.7618295855768338</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -5160,10 +5156,10 @@
         <v>15</v>
       </c>
       <c r="I38">
-        <v>361.29827057252191</v>
+        <v>361.73206703357096</v>
       </c>
       <c r="J38">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -5192,10 +5188,10 @@
         <v>25</v>
       </c>
       <c r="I39">
-        <v>361.33440039957918</v>
+        <v>361.76824024027434</v>
       </c>
       <c r="J39">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -5224,10 +5220,10 @@
         <v>13</v>
       </c>
       <c r="I40">
-        <v>361.37053383961916</v>
+        <v>361.80441706429838</v>
       </c>
       <c r="J40">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -5256,10 +5252,10 @@
         <v>1</v>
       </c>
       <c r="I41">
-        <v>361.40667089300314</v>
+        <v>361.84059750600483</v>
       </c>
       <c r="J41">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -5288,10 +5284,10 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>361.44281156009242</v>
+        <v>361.87678156575544</v>
       </c>
       <c r="J42">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -5320,10 +5316,10 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>361.47895584124842</v>
+        <v>361.91296924391202</v>
       </c>
       <c r="J43">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -5352,10 +5348,10 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>361.51510373683254</v>
+        <v>361.94916054083643</v>
       </c>
       <c r="J44">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -5384,10 +5380,10 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>361.5512552472062</v>
+        <v>361.98535545689049</v>
       </c>
       <c r="J45">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -5416,10 +5412,10 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>361.58741037273091</v>
+        <v>362.02155399243617</v>
       </c>
       <c r="J46">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -5448,10 +5444,10 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>361.62356911376816</v>
+        <v>362.05775614783539</v>
       </c>
       <c r="J47">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -5480,10 +5476,10 @@
         <v>10</v>
       </c>
       <c r="I48">
-        <v>361.6597314706795</v>
+        <v>362.09396192345019</v>
       </c>
       <c r="J48">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -5512,10 +5508,10 @@
         <v>18</v>
       </c>
       <c r="I49">
-        <v>361.6958974438266</v>
+        <v>362.13017131964256</v>
       </c>
       <c r="J49">
-        <v>-7.7618295855768338</v>
+        <v>-7.7910680778916674</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -5544,10 +5540,10 @@
         <v>26</v>
       </c>
       <c r="I50">
-        <v>361.73206703357096</v>
+        <v>362.16638433677451</v>
       </c>
       <c r="J50">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -5576,10 +5572,10 @@
         <v>20</v>
       </c>
       <c r="I51">
-        <v>361.76824024027434</v>
+        <v>362.20260097520821</v>
       </c>
       <c r="J51">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -5608,10 +5604,10 @@
         <v>22</v>
       </c>
       <c r="I52">
-        <v>361.80441706429838</v>
+        <v>362.23882123530575</v>
       </c>
       <c r="J52">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -5640,10 +5636,10 @@
         <v>2</v>
       </c>
       <c r="I53">
-        <v>361.84059750600483</v>
+        <v>362.27504511742927</v>
       </c>
       <c r="J53">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -5672,10 +5668,10 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>361.87678156575544</v>
+        <v>362.31127262194099</v>
       </c>
       <c r="J54">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -5704,10 +5700,10 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <v>361.91296924391202</v>
+        <v>362.34750374920316</v>
       </c>
       <c r="J55">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -5736,10 +5732,10 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>361.94916054083643</v>
+        <v>362.3837384995781</v>
       </c>
       <c r="J56">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -5768,10 +5764,10 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>361.98535545689049</v>
+        <v>362.41997687342803</v>
       </c>
       <c r="J57">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -5800,10 +5796,10 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>362.02155399243617</v>
+        <v>362.45621887111537</v>
       </c>
       <c r="J58">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -5832,10 +5828,10 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>362.05775614783539</v>
+        <v>362.4924644930025</v>
       </c>
       <c r="J59">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -5864,10 +5860,10 @@
         <v>1</v>
       </c>
       <c r="I60">
-        <v>362.09396192345019</v>
+        <v>362.5287137394518</v>
       </c>
       <c r="J60">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -5896,10 +5892,10 @@
         <v>11</v>
       </c>
       <c r="I61">
-        <v>362.13017131964256</v>
+        <v>362.56496661082576</v>
       </c>
       <c r="J61">
-        <v>-7.7910680778916674</v>
+        <v>-7.820947979612547</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -5928,10 +5924,10 @@
         <v>8</v>
       </c>
       <c r="I62">
-        <v>362.16638433677451</v>
+        <v>362.60122310748682</v>
       </c>
       <c r="J62">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -5960,10 +5956,10 @@
         <v>12</v>
       </c>
       <c r="I63">
-        <v>362.20260097520821</v>
+        <v>362.63748322979757</v>
       </c>
       <c r="J63">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -5992,10 +5988,10 @@
         <v>4</v>
       </c>
       <c r="I64">
-        <v>362.23882123530575</v>
+        <v>362.67374697812056</v>
       </c>
       <c r="J64">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -6024,10 +6020,10 @@
         <v>1</v>
       </c>
       <c r="I65">
-        <v>362.27504511742927</v>
+        <v>362.71001435281835</v>
       </c>
       <c r="J65">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -6056,10 +6052,10 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <v>362.31127262194099</v>
+        <v>362.74628535425364</v>
       </c>
       <c r="J66">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -6088,10 +6084,10 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <v>362.34750374920316</v>
+        <v>362.78255998278905</v>
       </c>
       <c r="J67">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -6120,10 +6116,10 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>362.3837384995781</v>
+        <v>362.81883823878735</v>
       </c>
       <c r="J68">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -6152,10 +6148,10 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <v>362.41997687342803</v>
+        <v>362.8551201226112</v>
       </c>
       <c r="J69">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -6184,10 +6180,10 @@
         <v>0</v>
       </c>
       <c r="I70">
-        <v>362.45621887111537</v>
+        <v>362.89140563462348</v>
       </c>
       <c r="J70">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -6216,10 +6212,10 @@
         <v>0</v>
       </c>
       <c r="I71">
-        <v>362.4924644930025</v>
+        <v>362.92769477518692</v>
       </c>
       <c r="J71">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -6248,10 +6244,10 @@
         <v>10</v>
       </c>
       <c r="I72">
-        <v>362.5287137394518</v>
+        <v>362.96398754466446</v>
       </c>
       <c r="J72">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -6280,10 +6276,10 @@
         <v>18</v>
       </c>
       <c r="I73">
-        <v>362.56496661082576</v>
+        <v>363.00028394341894</v>
       </c>
       <c r="J73">
-        <v>-7.820947979612547</v>
+        <v>-7.8514833614385262</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -6312,10 +6308,10 @@
         <v>10</v>
       </c>
       <c r="I74">
-        <v>362.60122310748682</v>
+        <v>363.03658397181329</v>
       </c>
       <c r="J74">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -6344,10 +6340,10 @@
         <v>17</v>
       </c>
       <c r="I75">
-        <v>362.63748322979757</v>
+        <v>363.07288763021046</v>
       </c>
       <c r="J75">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -6376,10 +6372,10 @@
         <v>10</v>
       </c>
       <c r="I76">
-        <v>362.67374697812056</v>
+        <v>363.10919491897346</v>
       </c>
       <c r="J76">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -6408,10 +6404,10 @@
         <v>3</v>
       </c>
       <c r="I77">
-        <v>362.71001435281835</v>
+        <v>363.14550583846534</v>
       </c>
       <c r="J77">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
@@ -6440,10 +6436,10 @@
         <v>0</v>
       </c>
       <c r="I78">
-        <v>362.74628535425364</v>
+        <v>363.18182038904916</v>
       </c>
       <c r="J78">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -6472,10 +6468,10 @@
         <v>0</v>
       </c>
       <c r="I79">
-        <v>362.78255998278905</v>
+        <v>363.21813857108805</v>
       </c>
       <c r="J79">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
@@ -6504,10 +6500,10 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <v>362.81883823878735</v>
+        <v>363.25446038494516</v>
       </c>
       <c r="J80">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -6536,10 +6532,10 @@
         <v>0</v>
       </c>
       <c r="I81">
-        <v>362.8551201226112</v>
+        <v>363.29078583098368</v>
       </c>
       <c r="J81">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -6568,10 +6564,10 @@
         <v>0</v>
       </c>
       <c r="I82">
-        <v>362.89140563462348</v>
+        <v>363.32711490956677</v>
       </c>
       <c r="J82">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
@@ -6600,10 +6596,10 @@
         <v>1</v>
       </c>
       <c r="I83">
-        <v>362.92769477518692</v>
+        <v>363.36344762105773</v>
       </c>
       <c r="J83">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
@@ -6632,10 +6628,10 @@
         <v>11</v>
       </c>
       <c r="I84">
-        <v>362.96398754466446</v>
+        <v>363.39978396581984</v>
       </c>
       <c r="J84">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
@@ -6664,10 +6660,10 @@
         <v>19</v>
       </c>
       <c r="I85">
-        <v>363.00028394341894</v>
+        <v>363.43612394421643</v>
       </c>
       <c r="J85">
-        <v>-7.8514833614385262</v>
+        <v>-7.8826886027397975</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -6696,10 +6692,10 @@
         <v>29</v>
       </c>
       <c r="I86">
-        <v>363.03658397181329</v>
+        <v>363.47246755661087</v>
       </c>
       <c r="J86">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
@@ -6728,10 +6724,10 @@
         <v>22</v>
       </c>
       <c r="I87">
-        <v>363.07288763021046</v>
+        <v>363.50881480336653</v>
       </c>
       <c r="J87">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
@@ -6760,10 +6756,10 @@
         <v>9</v>
       </c>
       <c r="I88">
-        <v>363.10919491897346</v>
+        <v>363.54516568484689</v>
       </c>
       <c r="J88">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -6792,10 +6788,10 @@
         <v>0</v>
       </c>
       <c r="I89">
-        <v>363.14550583846534</v>
+        <v>363.5815202014154</v>
       </c>
       <c r="J89">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
@@ -6824,10 +6820,10 @@
         <v>0</v>
       </c>
       <c r="I90">
-        <v>363.18182038904916</v>
+        <v>363.61787835343551</v>
       </c>
       <c r="J90">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
@@ -6856,10 +6852,10 @@
         <v>0</v>
       </c>
       <c r="I91">
-        <v>363.21813857108805</v>
+        <v>363.65424014127086</v>
       </c>
       <c r="J91">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -6888,10 +6884,10 @@
         <v>0</v>
       </c>
       <c r="I92">
-        <v>363.25446038494516</v>
+        <v>363.69060556528501</v>
       </c>
       <c r="J92">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
@@ -6920,10 +6916,10 @@
         <v>0</v>
       </c>
       <c r="I93">
-        <v>363.29078583098368</v>
+        <v>363.72697462584154</v>
       </c>
       <c r="J93">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
@@ -6952,10 +6948,10 @@
         <v>0</v>
       </c>
       <c r="I94">
-        <v>363.32711490956677</v>
+        <v>363.76334732330412</v>
       </c>
       <c r="J94">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
@@ -6984,10 +6980,10 @@
         <v>2</v>
       </c>
       <c r="I95">
-        <v>363.36344762105773</v>
+        <v>363.79972365803644</v>
       </c>
       <c r="J95">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
@@ -7016,10 +7012,10 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <v>363.39978396581984</v>
+        <v>363.83610363040225</v>
       </c>
       <c r="J96">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
@@ -7048,10 +7044,10 @@
         <v>16</v>
       </c>
       <c r="I97">
-        <v>363.43612394421643</v>
+        <v>363.87248724076528</v>
       </c>
       <c r="J97">
-        <v>-7.8826886027397975</v>
+        <v>-7.9145783983290627</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
@@ -7080,10 +7076,10 @@
         <v>29</v>
       </c>
       <c r="I98">
-        <v>363.47246755661087</v>
+        <v>363.90887448948934</v>
       </c>
       <c r="J98">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -7112,10 +7108,10 @@
         <v>22</v>
       </c>
       <c r="I99">
-        <v>363.50881480336653</v>
+        <v>363.94526537693827</v>
       </c>
       <c r="J99">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
@@ -7144,10 +7140,10 @@
         <v>15</v>
       </c>
       <c r="I100">
-        <v>363.54516568484689</v>
+        <v>363.98165990347593</v>
       </c>
       <c r="J100">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -7176,10 +7172,10 @@
         <v>2</v>
       </c>
       <c r="I101">
-        <v>363.5815202014154</v>
+        <v>364.01805806946629</v>
       </c>
       <c r="J101">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -7208,10 +7204,10 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <v>363.61787835343551</v>
+        <v>364.05445987527321</v>
       </c>
       <c r="J102">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -7240,10 +7236,10 @@
         <v>0</v>
       </c>
       <c r="I103">
-        <v>363.65424014127086</v>
+        <v>364.09086532126071</v>
       </c>
       <c r="J103">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
@@ -7272,10 +7268,10 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <v>363.69060556528501</v>
+        <v>364.12727440779281</v>
       </c>
       <c r="J104">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
@@ -7304,10 +7300,10 @@
         <v>0</v>
       </c>
       <c r="I105">
-        <v>363.72697462584154</v>
+        <v>364.1636871352336</v>
       </c>
       <c r="J105">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
@@ -7336,10 +7332,10 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <v>363.76334732330412</v>
+        <v>364.2001035039471</v>
       </c>
       <c r="J106">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -7368,10 +7364,10 @@
         <v>4</v>
       </c>
       <c r="I107">
-        <v>363.79972365803644</v>
+        <v>364.23652351429752</v>
       </c>
       <c r="J107">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
@@ -7400,10 +7396,10 @@
         <v>5</v>
       </c>
       <c r="I108">
-        <v>363.83610363040225</v>
+        <v>364.27294716664892</v>
       </c>
       <c r="J108">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -7432,10 +7428,10 @@
         <v>30</v>
       </c>
       <c r="I109">
-        <v>363.87248724076528</v>
+        <v>364.30937446136556</v>
       </c>
       <c r="J109">
-        <v>-7.9145783983290627</v>
+        <v>-7.9471677653814368</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
@@ -7464,10 +7460,10 @@
         <v>20</v>
       </c>
       <c r="I110">
-        <v>363.90887448948934</v>
+        <v>364.34580539881171</v>
       </c>
       <c r="J110">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -7496,10 +7492,10 @@
         <v>20</v>
       </c>
       <c r="I111">
-        <v>363.94526537693827</v>
+        <v>364.3822399793516</v>
       </c>
       <c r="J111">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
@@ -7528,10 +7524,10 @@
         <v>12</v>
       </c>
       <c r="I112">
-        <v>363.98165990347593</v>
+        <v>364.41867820334954</v>
       </c>
       <c r="J112">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
@@ -7560,10 +7556,10 @@
         <v>0</v>
       </c>
       <c r="I113">
-        <v>364.01805806946629</v>
+        <v>364.45512007116986</v>
       </c>
       <c r="J113">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -7592,10 +7588,10 @@
         <v>0</v>
       </c>
       <c r="I114">
-        <v>364.05445987527321</v>
+        <v>364.49156558317696</v>
       </c>
       <c r="J114">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
@@ -7624,10 +7620,10 @@
         <v>0</v>
       </c>
       <c r="I115">
-        <v>364.09086532126071</v>
+        <v>364.52801473973528</v>
       </c>
       <c r="J115">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -7656,10 +7652,10 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <v>364.12727440779281</v>
+        <v>364.56446754120924</v>
       </c>
       <c r="J116">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
@@ -7688,10 +7684,10 @@
         <v>0</v>
       </c>
       <c r="I117">
-        <v>364.1636871352336</v>
+        <v>364.60092398796337</v>
       </c>
       <c r="J117">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
@@ -7720,10 +7716,10 @@
         <v>0</v>
       </c>
       <c r="I118">
-        <v>364.2001035039471</v>
+        <v>364.63738408036215</v>
       </c>
       <c r="J118">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
@@ -7752,10 +7748,10 @@
         <v>3</v>
       </c>
       <c r="I119">
-        <v>364.23652351429752</v>
+        <v>364.67384781877018</v>
       </c>
       <c r="J119">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
@@ -7784,10 +7780,10 @@
         <v>14</v>
       </c>
       <c r="I120">
-        <v>364.27294716664892</v>
+        <v>364.71031520355206</v>
       </c>
       <c r="J120">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
@@ -7816,10 +7812,10 @@
         <v>6</v>
       </c>
       <c r="I121">
-        <v>364.30937446136556</v>
+        <v>364.74678623507242</v>
       </c>
       <c r="J121">
-        <v>-7.9471677653814368</v>
+        <v>-7.9804720505061724</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
@@ -7848,10 +7844,10 @@
         <v>13</v>
       </c>
       <c r="I122">
-        <v>364.34580539881171</v>
+        <v>364.78326091369593</v>
       </c>
       <c r="J122">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
@@ -7880,10 +7876,10 @@
         <v>19</v>
       </c>
       <c r="I123">
-        <v>364.3822399793516</v>
+        <v>364.81973923978728</v>
       </c>
       <c r="J123">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
@@ -7912,10 +7908,10 @@
         <v>8</v>
       </c>
       <c r="I124">
-        <v>364.41867820334954</v>
+        <v>364.85622121371125</v>
       </c>
       <c r="J124">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -7944,10 +7940,10 @@
         <v>4</v>
       </c>
       <c r="I125">
-        <v>364.45512007116986</v>
+        <v>364.8927068358326</v>
       </c>
       <c r="J125">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
@@ -7976,10 +7972,10 @@
         <v>0</v>
       </c>
       <c r="I126">
-        <v>364.49156558317696</v>
+        <v>364.9291961065162</v>
       </c>
       <c r="J126">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
@@ -8008,10 +8004,10 @@
         <v>0</v>
       </c>
       <c r="I127">
-        <v>364.52801473973528</v>
+        <v>364.96568902612682</v>
       </c>
       <c r="J127">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
@@ -8040,10 +8036,10 @@
         <v>0</v>
       </c>
       <c r="I128">
-        <v>364.56446754120924</v>
+        <v>365.00218559502946</v>
       </c>
       <c r="J128">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
@@ -8072,10 +8068,10 @@
         <v>0</v>
       </c>
       <c r="I129">
-        <v>364.60092398796337</v>
+        <v>365.03868581358898</v>
       </c>
       <c r="J129">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
@@ -8104,10 +8100,10 @@
         <v>0</v>
       </c>
       <c r="I130">
-        <v>364.63738408036215</v>
+        <v>365.07518968217033</v>
       </c>
       <c r="J130">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
@@ -8136,10 +8132,10 @@
         <v>2</v>
       </c>
       <c r="I131">
-        <v>364.67384781877018</v>
+        <v>365.11169720113855</v>
       </c>
       <c r="J131">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
@@ -8168,10 +8164,10 @@
         <v>8</v>
       </c>
       <c r="I132">
-        <v>364.71031520355206</v>
+        <v>365.14820837085864</v>
       </c>
       <c r="J132">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
@@ -8200,10 +8196,10 @@
         <v>14</v>
       </c>
       <c r="I133">
-        <v>364.74678623507242</v>
+        <v>365.1847231916957</v>
       </c>
       <c r="J133">
-        <v>-7.9804720505061724</v>
+        <v>-8.0145069369735005</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
@@ -8232,10 +8228,10 @@
         <v>18</v>
       </c>
       <c r="I134">
-        <v>364.78326091369593</v>
+        <v>365.22124166401488</v>
       </c>
       <c r="J134">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
@@ -8264,10 +8260,10 @@
         <v>26</v>
       </c>
       <c r="I135">
-        <v>364.81973923978728</v>
+        <v>365.25776378818131</v>
       </c>
       <c r="J135">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
@@ -8296,10 +8292,10 @@
         <v>26</v>
       </c>
       <c r="I136">
-        <v>364.85622121371125</v>
+        <v>365.29428956456013</v>
       </c>
       <c r="J136">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
@@ -8328,10 +8324,10 @@
         <v>7</v>
       </c>
       <c r="I137">
-        <v>364.8927068358326</v>
+        <v>365.33081899351657</v>
       </c>
       <c r="J137">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
@@ -8360,10 +8356,10 @@
         <v>0</v>
       </c>
       <c r="I138">
-        <v>364.9291961065162</v>
+        <v>365.36735207541591</v>
       </c>
       <c r="J138">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
@@ -8392,10 +8388,10 @@
         <v>0</v>
       </c>
       <c r="I139">
-        <v>364.96568902612682</v>
+        <v>365.40388881062347</v>
       </c>
       <c r="J139">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
@@ -8424,10 +8420,10 @@
         <v>0</v>
       </c>
       <c r="I140">
-        <v>365.00218559502946</v>
+        <v>365.44042919950454</v>
       </c>
       <c r="J140">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
@@ -8456,10 +8452,10 @@
         <v>0</v>
       </c>
       <c r="I141">
-        <v>365.03868581358898</v>
+        <v>365.47697324242449</v>
       </c>
       <c r="J141">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
@@ -8488,10 +8484,10 @@
         <v>0</v>
       </c>
       <c r="I142">
-        <v>365.07518968217033</v>
+        <v>365.51352093974873</v>
       </c>
       <c r="J142">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
@@ -8520,10 +8516,10 @@
         <v>1</v>
       </c>
       <c r="I143">
-        <v>365.11169720113855</v>
+        <v>365.5500722918427</v>
       </c>
       <c r="J143">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -8552,10 +8548,10 @@
         <v>8</v>
       </c>
       <c r="I144">
-        <v>365.14820837085864</v>
+        <v>365.58662729907189</v>
       </c>
       <c r="J144">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -8584,10 +8580,10 @@
         <v>11</v>
       </c>
       <c r="I145">
-        <v>365.1847231916957</v>
+        <v>365.62318596180182</v>
       </c>
       <c r="J145">
-        <v>-8.0145069369735005</v>
+        <v>-8.0492884521000221</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
@@ -8616,10 +8612,10 @@
         <v>10</v>
       </c>
       <c r="I146">
-        <v>365.22124166401488</v>
+        <v>365.65974828039799</v>
       </c>
       <c r="J146">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
@@ -8648,10 +8644,10 @@
         <v>7</v>
       </c>
       <c r="I147">
-        <v>365.25776378818131</v>
+        <v>365.69631425522601</v>
       </c>
       <c r="J147">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
@@ -8680,10 +8676,10 @@
         <v>5</v>
       </c>
       <c r="I148">
-        <v>365.29428956456013</v>
+        <v>365.73288388665151</v>
       </c>
       <c r="J148">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
@@ -8712,10 +8708,10 @@
         <v>0</v>
       </c>
       <c r="I149">
-        <v>365.33081899351657</v>
+        <v>365.76945717504015</v>
       </c>
       <c r="J149">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
@@ -8744,10 +8740,10 @@
         <v>0</v>
       </c>
       <c r="I150">
-        <v>365.36735207541591</v>
+        <v>365.80603412075766</v>
       </c>
       <c r="J150">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
@@ -8776,10 +8772,10 @@
         <v>0</v>
       </c>
       <c r="I151">
-        <v>365.40388881062347</v>
+        <v>365.84261472416972</v>
       </c>
       <c r="J151">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
@@ -8808,10 +8804,10 @@
         <v>0</v>
       </c>
       <c r="I152">
-        <v>365.44042919950454</v>
+        <v>365.87919898564212</v>
       </c>
       <c r="J152">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
@@ -8840,10 +8836,10 @@
         <v>0</v>
       </c>
       <c r="I153">
-        <v>365.47697324242449</v>
+        <v>365.9157869055407</v>
       </c>
       <c r="J153">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
@@ -8872,10 +8868,10 @@
         <v>0</v>
       </c>
       <c r="I154">
-        <v>365.51352093974873</v>
+        <v>365.95237848423125</v>
       </c>
       <c r="J154">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
@@ -8904,10 +8900,10 @@
         <v>0</v>
       </c>
       <c r="I155">
-        <v>365.5500722918427</v>
+        <v>365.98897372207966</v>
       </c>
       <c r="J155">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
@@ -8936,10 +8932,10 @@
         <v>4</v>
       </c>
       <c r="I156">
-        <v>365.58662729907189</v>
+        <v>366.02557261945185</v>
       </c>
       <c r="J156">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
@@ -8968,10 +8964,10 @@
         <v>11</v>
       </c>
       <c r="I157">
-        <v>365.62318596180182</v>
+        <v>366.06217517671377</v>
       </c>
       <c r="J157">
-        <v>-8.0492884521000221</v>
+        <v>-8.0848329747961003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
development routins, not needed
</commit_message>
<xml_diff>
--- a/dev/input_data/input_eu_mixed.xlsx
+++ b/dev/input_data/input_eu_mixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D220B0B-9939-C24F-8542-07FFA896AAE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F6B2B2-CACF-3B4F-839A-588F0F7CA21F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="4" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
+    <workbookView xWindow="24800" yWindow="560" windowWidth="25020" windowHeight="28120" activeTab="1" xr2:uid="{61EEFE5B-6AE1-A641-A9AB-273DC4213F59}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1114,7 +1114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1467,13 +1467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003E9A71-E1A2-2845-B4A9-990606FB2D91}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1483,7 +1483,7 @@
     <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>323</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>0.1259168645351276</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>2.2679</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>4.2920969347823963</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>4.2920969347823963</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>0.38277020142713869</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>0.39457142857142857</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>128</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>131</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>4.8565574202227367E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>151</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>154</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>160</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>163</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>166</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>169</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>172</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>178</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>181</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -2723,77 +2723,411 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>310</v>
+        <v>184</v>
       </c>
       <c r="B63" t="s">
-        <v>311</v>
+        <v>185</v>
       </c>
       <c r="C63" t="s">
-        <v>311</v>
+        <v>185</v>
       </c>
       <c r="D63" t="s">
-        <v>312</v>
+        <v>6</v>
       </c>
       <c r="E63">
-        <v>-90</v>
-      </c>
-      <c r="F63" s="1">
-        <v>-90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.0079269437862552</v>
+      </c>
+      <c r="F63">
+        <v>4.588685316132576</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>313</v>
+        <v>186</v>
       </c>
       <c r="B64" t="s">
-        <v>314</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>314</v>
+        <v>187</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
       <c r="E64">
+        <v>0.53753519999999999</v>
+      </c>
+      <c r="F64">
+        <v>0.4738211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65">
+        <v>0.44984780000000002</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" t="s">
+        <v>193</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>194</v>
+      </c>
+      <c r="B68" t="s">
+        <v>195</v>
+      </c>
+      <c r="C68" t="s">
+        <v>195</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>196</v>
+      </c>
+      <c r="B69" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" t="s">
+        <v>197</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B70" t="s">
+        <v>201</v>
+      </c>
+      <c r="C70" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>0.93895242486246377</v>
+      </c>
+      <c r="F70">
+        <v>1.3764906078875401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>202</v>
+      </c>
+      <c r="B71" t="s">
+        <v>203</v>
+      </c>
+      <c r="C71" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71">
+        <v>0.5812155</v>
+      </c>
+      <c r="F71">
+        <v>0.55362769999999994</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>204</v>
+      </c>
+      <c r="B72" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" t="s">
+        <v>205</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>206</v>
+      </c>
+      <c r="B73" t="s">
+        <v>207</v>
+      </c>
+      <c r="C73" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>-0.27724310000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>208</v>
+      </c>
+      <c r="B74" t="s">
+        <v>209</v>
+      </c>
+      <c r="C74" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" t="s">
+        <v>211</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75">
+        <v>6.2690037344620873</v>
+      </c>
+      <c r="F75">
+        <v>2.1885791577597868</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>212</v>
+      </c>
+      <c r="B76" t="s">
+        <v>213</v>
+      </c>
+      <c r="C76" t="s">
+        <v>213</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76">
+        <v>0.18916359999999999</v>
+      </c>
+      <c r="F76">
+        <v>0.56325259999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" t="s">
+        <v>215</v>
+      </c>
+      <c r="C77" t="s">
+        <v>215</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>216</v>
+      </c>
+      <c r="B78" t="s">
+        <v>217</v>
+      </c>
+      <c r="C78" t="s">
+        <v>217</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>-0.26567479999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" t="s">
+        <v>219</v>
+      </c>
+      <c r="C79" t="s">
+        <v>219</v>
+      </c>
+      <c r="E79">
+        <v>0.6551283</v>
+      </c>
+      <c r="F79">
+        <v>0.67789920000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>310</v>
+      </c>
+      <c r="B80" t="s">
+        <v>311</v>
+      </c>
+      <c r="C80" t="s">
+        <v>311</v>
+      </c>
+      <c r="D80" t="s">
+        <v>312</v>
+      </c>
+      <c r="E80">
+        <v>-90</v>
+      </c>
+      <c r="F80" s="1">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>313</v>
+      </c>
+      <c r="B81" t="s">
+        <v>314</v>
+      </c>
+      <c r="C81" t="s">
+        <v>314</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81">
         <v>0.8</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F81" s="1">
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
         <v>315</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B82" t="s">
         <v>316</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D82" t="s">
         <v>317</v>
       </c>
-      <c r="E65">
+      <c r="E82">
         <v>24</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F82" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
         <v>318</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B83" t="s">
         <v>319</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D83" t="s">
         <v>320</v>
       </c>
-      <c r="E66">
+      <c r="E83">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F83" s="1">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -2804,15 +3138,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB4F449-9DC8-E74B-BCC1-554BB33610F9}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>323</v>
       </c>
@@ -2832,95 +3166,95 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2">
-        <v>1.0079269437862552</v>
+        <v>0.19438798391558637</v>
       </c>
       <c r="F2">
-        <v>4.588685316132576</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.27800157495549827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3">
-        <v>0.53753519999999999</v>
+        <v>1.2246192</v>
       </c>
       <c r="F3">
-        <v>0.4738211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.1518027</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4">
-        <v>0.44984780000000002</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.12776940000000001</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -2929,825 +3263,491 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5.4277699999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.78810101950457778</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.2283156000459392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.31619239999999998</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9">
-        <v>0.93895242486246377</v>
+        <v>1.6142477</v>
       </c>
       <c r="F9">
-        <v>1.3764906078875401</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.1889634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>246</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10">
-        <v>0.5812155</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.55362769999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-0.11702410000000001</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.2143678</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="C12" t="s">
-        <v>207</v>
+        <v>252</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1.6360918833167544</v>
       </c>
       <c r="F12">
-        <v>-0.27724310000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.98723714491917658</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
-        <v>209</v>
+        <v>255</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.50466180000000005</v>
       </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.87204890000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>258</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14">
-        <v>6.2690037344620873</v>
+        <v>-0.62634160000000005</v>
       </c>
       <c r="F14">
-        <v>2.1885791577597868</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.25852E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15">
-        <v>0.18916359999999999</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.56325259999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
       <c r="C16" t="s">
-        <v>215</v>
+        <v>264</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>4.5786399999999998E-2</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.10617219999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>265</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>266</v>
       </c>
       <c r="C17" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2.2094402126214635E-2</v>
       </c>
       <c r="F17">
-        <v>-0.26567479999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9.0008110144060058E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>218</v>
+        <v>268</v>
       </c>
       <c r="B18" t="s">
-        <v>219</v>
+        <v>269</v>
       </c>
       <c r="C18" t="s">
-        <v>219</v>
+        <v>270</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>0.6551283</v>
+        <v>2.6048110000000002</v>
       </c>
       <c r="F18">
-        <v>0.67789920000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.0841154999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
       <c r="C19" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19">
-        <v>0.19438798391558637</v>
+        <v>-1.8148740000000001</v>
       </c>
       <c r="F19">
-        <v>0.27800157495549827</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>274</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>276</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20">
-        <v>1.2246192</v>
+        <v>0.32097799999999999</v>
       </c>
       <c r="F20">
-        <v>1.1518027</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.27149630000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>277</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>278</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>8.9823E-2</v>
       </c>
       <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.1222255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>280</v>
       </c>
       <c r="B22" t="s">
-        <v>230</v>
+        <v>281</v>
       </c>
       <c r="C22" t="s">
-        <v>231</v>
+        <v>282</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22">
-        <v>0.12776940000000001</v>
+        <v>0.64586569454210141</v>
       </c>
       <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.1339352444324555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="B23" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="C23" t="s">
-        <v>234</v>
+        <v>285</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.26870719999999998</v>
       </c>
       <c r="F23">
-        <v>5.4277699999999998E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>235</v>
+        <v>286</v>
       </c>
       <c r="B24" t="s">
-        <v>236</v>
+        <v>287</v>
       </c>
       <c r="C24" t="s">
-        <v>237</v>
+        <v>288</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
       <c r="E24">
-        <v>0.78810101950457778</v>
+        <v>1.7403652999999999</v>
       </c>
       <c r="F24">
-        <v>1.2283156000459392</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.94494829999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>238</v>
+        <v>289</v>
       </c>
       <c r="B25" t="s">
-        <v>239</v>
+        <v>290</v>
       </c>
       <c r="C25" t="s">
-        <v>240</v>
+        <v>291</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
       <c r="E25">
-        <v>0.31619239999999998</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
+        <v>293</v>
       </c>
       <c r="C26" t="s">
-        <v>243</v>
+        <v>294</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26">
-        <v>1.6142477</v>
+        <v>-0.14293220000000001</v>
       </c>
       <c r="F26">
-        <v>1.1889634</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.12202789999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>244</v>
+        <v>295</v>
       </c>
       <c r="B27" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
       <c r="C27" t="s">
-        <v>246</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
+        <v>297</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.14272679508242667</v>
       </c>
       <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.22778889000228159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>247</v>
+        <v>298</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>299</v>
       </c>
       <c r="C28" t="s">
-        <v>249</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
+        <v>300</v>
       </c>
       <c r="E28">
-        <v>-0.11702410000000001</v>
+        <v>1.028025</v>
       </c>
       <c r="F28">
-        <v>0.2143678</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.203662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="C29" t="s">
-        <v>252</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
+        <v>303</v>
       </c>
       <c r="E29">
-        <v>1.6360918833167544</v>
+        <v>-3.4997509999999998</v>
       </c>
       <c r="F29">
-        <v>0.98723714491917658</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="B30" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
       <c r="C30" t="s">
-        <v>255</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
+        <v>306</v>
       </c>
       <c r="E30">
-        <v>0.50466180000000005</v>
+        <v>0.453181</v>
       </c>
       <c r="F30">
-        <v>0.87204890000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.41872100000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="B31" t="s">
-        <v>257</v>
+        <v>308</v>
       </c>
       <c r="C31" t="s">
-        <v>258</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
+        <v>309</v>
       </c>
       <c r="E31">
-        <v>-0.62634160000000005</v>
+        <v>0.20796600000000001</v>
       </c>
       <c r="F31">
-        <v>2.25852E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>259</v>
-      </c>
-      <c r="B32" t="s">
-        <v>260</v>
-      </c>
-      <c r="C32" t="s">
-        <v>261</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>262</v>
-      </c>
-      <c r="B33" t="s">
-        <v>263</v>
-      </c>
-      <c r="C33" t="s">
-        <v>264</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33">
-        <v>4.5786399999999998E-2</v>
-      </c>
-      <c r="F33">
-        <v>-0.10617219999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>265</v>
-      </c>
-      <c r="B34" t="s">
-        <v>266</v>
-      </c>
-      <c r="C34" t="s">
-        <v>267</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34">
-        <v>2.2094402126214635E-2</v>
-      </c>
-      <c r="F34">
-        <v>9.0008110144060058E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>268</v>
-      </c>
-      <c r="B35" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" t="s">
-        <v>270</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <v>2.6048110000000002</v>
-      </c>
-      <c r="F35">
-        <v>2.0841154999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>271</v>
-      </c>
-      <c r="B36" t="s">
-        <v>272</v>
-      </c>
-      <c r="C36" t="s">
-        <v>273</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36">
-        <v>-1.8148740000000001</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>274</v>
-      </c>
-      <c r="B37" t="s">
-        <v>275</v>
-      </c>
-      <c r="C37" t="s">
-        <v>276</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37">
-        <v>0.32097799999999999</v>
-      </c>
-      <c r="F37">
-        <v>0.27149630000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>277</v>
-      </c>
-      <c r="B38" t="s">
-        <v>278</v>
-      </c>
-      <c r="C38" t="s">
-        <v>279</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38">
-        <v>8.9823E-2</v>
-      </c>
-      <c r="F38">
-        <v>-0.1222255</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>280</v>
-      </c>
-      <c r="B39" t="s">
-        <v>281</v>
-      </c>
-      <c r="C39" t="s">
-        <v>282</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39">
-        <v>0.64586569454210141</v>
-      </c>
-      <c r="F39">
-        <v>1.1339352444324555</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>283</v>
-      </c>
-      <c r="B40" t="s">
-        <v>284</v>
-      </c>
-      <c r="C40" t="s">
-        <v>285</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40">
-        <v>0.26870719999999998</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>286</v>
-      </c>
-      <c r="B41" t="s">
-        <v>287</v>
-      </c>
-      <c r="C41" t="s">
-        <v>288</v>
-      </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41">
-        <v>1.7403652999999999</v>
-      </c>
-      <c r="F41">
-        <v>0.94494829999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>289</v>
-      </c>
-      <c r="B42" t="s">
-        <v>290</v>
-      </c>
-      <c r="C42" t="s">
-        <v>291</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>292</v>
-      </c>
-      <c r="B43" t="s">
-        <v>293</v>
-      </c>
-      <c r="C43" t="s">
-        <v>294</v>
-      </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43">
-        <v>-0.14293220000000001</v>
-      </c>
-      <c r="F43">
-        <v>0.12202789999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>295</v>
-      </c>
-      <c r="B44" t="s">
-        <v>296</v>
-      </c>
-      <c r="C44" t="s">
-        <v>297</v>
-      </c>
-      <c r="E44">
-        <v>0.14272679508242667</v>
-      </c>
-      <c r="F44">
-        <v>0.22778889000228159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>298</v>
-      </c>
-      <c r="B45" t="s">
-        <v>299</v>
-      </c>
-      <c r="C45" t="s">
-        <v>300</v>
-      </c>
-      <c r="E45">
-        <v>1.028025</v>
-      </c>
-      <c r="F45">
-        <v>2.203662</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>301</v>
-      </c>
-      <c r="B46" t="s">
-        <v>302</v>
-      </c>
-      <c r="C46" t="s">
-        <v>303</v>
-      </c>
-      <c r="E46">
-        <v>-3.4997509999999998</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>304</v>
-      </c>
-      <c r="B47" t="s">
-        <v>305</v>
-      </c>
-      <c r="C47" t="s">
-        <v>306</v>
-      </c>
-      <c r="E47">
-        <v>0.453181</v>
-      </c>
-      <c r="F47">
-        <v>-0.41872100000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>307</v>
-      </c>
-      <c r="B48" t="s">
-        <v>308</v>
-      </c>
-      <c r="C48" t="s">
-        <v>309</v>
-      </c>
-      <c r="E48">
-        <v>0.20796600000000001</v>
-      </c>
-      <c r="F48">
         <v>0</v>
       </c>
     </row>
@@ -3764,7 +3764,7 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3783,7 +3783,7 @@
     <col min="15" max="15" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>325</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>50.11353888888889</v>
       </c>
@@ -3848,12 +3848,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>324</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>321</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="19" customHeight="1">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -3940,13 +3940,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E86F09-F9D3-4B49-968A-3E0A41AAD9D8}">
   <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="M145" sqref="M145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>344</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>2002</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>2002</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>2002</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>2002</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2002</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>-7.7052220501109474</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>2003</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>2003</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>2003</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>2003</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>2003</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>2003</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>-7.7332187340141187</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>2004</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>2004</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>2004</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>2004</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>2004</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>2004</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>2004</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>2004</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>2004</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>2004</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>-7.7618295855768338</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>2005</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>2005</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>2005</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>2005</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>2005</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>2005</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>2005</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>2005</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>2005</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>2005</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>2005</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>2005</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>-7.7910680778916674</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>2006</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>2006</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>2006</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>2006</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>2006</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>2006</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>2006</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>2006</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>2006</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>2006</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>2006</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>2006</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>-7.820947979612547</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>2007</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>2007</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>2007</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>2007</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>2007</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>2007</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>2007</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>2007</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>2007</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>2007</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>2007</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>2007</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>-7.8514833614385262</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>2008</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>2008</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>2008</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>2008</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>2008</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>2008</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>2008</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>2008</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>2008</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>2008</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>2008</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>2008</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>-7.8826886027397975</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>2009</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>2009</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>2009</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>2009</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>2009</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>2009</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>2009</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>2009</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>2009</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>2009</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>2009</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>2009</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>-7.9145783983290627</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>2010</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>2010</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10">
       <c r="A100">
         <v>2010</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10">
       <c r="A101">
         <v>2010</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10">
       <c r="A102">
         <v>2010</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10">
       <c r="A103">
         <v>2010</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10">
       <c r="A104">
         <v>2010</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10">
       <c r="A105">
         <v>2010</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10">
       <c r="A106">
         <v>2010</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10">
       <c r="A107">
         <v>2010</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10">
       <c r="A108">
         <v>2010</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10">
       <c r="A109">
         <v>2010</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>-7.9471677653814368</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10">
       <c r="A110">
         <v>2011</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10">
       <c r="A111">
         <v>2011</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10">
       <c r="A112">
         <v>2011</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10">
       <c r="A113">
         <v>2011</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10">
       <c r="A114">
         <v>2011</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10">
       <c r="A115">
         <v>2011</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10">
       <c r="A116">
         <v>2011</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10">
       <c r="A117">
         <v>2011</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10">
       <c r="A118">
         <v>2011</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10">
       <c r="A119">
         <v>2011</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10">
       <c r="A120">
         <v>2011</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10">
       <c r="A121">
         <v>2011</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>-7.9804720505061724</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10">
       <c r="A122">
         <v>2012</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10">
       <c r="A123">
         <v>2012</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10">
       <c r="A124">
         <v>2012</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10">
       <c r="A125">
         <v>2012</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10">
       <c r="A126">
         <v>2012</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10">
       <c r="A127">
         <v>2012</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10">
       <c r="A128">
         <v>2012</v>
       </c>
@@ -8042,7 +8042,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10">
       <c r="A129">
         <v>2012</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10">
       <c r="A130">
         <v>2012</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10">
       <c r="A131">
         <v>2012</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10">
       <c r="A132">
         <v>2012</v>
       </c>
@@ -8170,7 +8170,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10">
       <c r="A133">
         <v>2012</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>-8.0145069369735005</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10">
       <c r="A134">
         <v>2013</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10">
       <c r="A135">
         <v>2013</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10">
       <c r="A136">
         <v>2013</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10">
       <c r="A137">
         <v>2013</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10">
       <c r="A138">
         <v>2013</v>
       </c>
@@ -8362,7 +8362,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10">
       <c r="A139">
         <v>2013</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10">
       <c r="A140">
         <v>2013</v>
       </c>
@@ -8426,7 +8426,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10">
       <c r="A141">
         <v>2013</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10">
       <c r="A142">
         <v>2013</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10">
       <c r="A143">
         <v>2013</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10">
       <c r="A144">
         <v>2013</v>
       </c>
@@ -8554,7 +8554,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10">
       <c r="A145">
         <v>2013</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>-8.0492884521000221</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10">
       <c r="A146">
         <v>2014</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10">
       <c r="A147">
         <v>2014</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10">
       <c r="A148">
         <v>2014</v>
       </c>
@@ -8682,7 +8682,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10">
       <c r="A149">
         <v>2014</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10">
       <c r="A150">
         <v>2014</v>
       </c>
@@ -8746,7 +8746,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10">
       <c r="A151">
         <v>2014</v>
       </c>
@@ -8778,7 +8778,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10">
       <c r="A152">
         <v>2014</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10">
       <c r="A153">
         <v>2014</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10">
       <c r="A154">
         <v>2014</v>
       </c>
@@ -8874,7 +8874,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10">
       <c r="A155">
         <v>2014</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10">
       <c r="A156">
         <v>2014</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>-8.0848329747961003</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10">
       <c r="A157">
         <v>2014</v>
       </c>
@@ -8983,9 +8983,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>336</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>342</v>
       </c>
@@ -9035,9 +9035,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>353</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>999</v>
       </c>

</xml_diff>